<commit_message>
feat: update Sound config
</commit_message>
<xml_diff>
--- a/Excel/Sound_音效表.xlsx
+++ b/Excel/Sound_音效表.xlsx
@@ -38,7 +38,7 @@
     <t>soundName</t>
   </si>
   <si>
-    <t>loopPlayBack</t>
+    <t>loopCount</t>
   </si>
   <si>
     <t>volume</t>
@@ -68,9 +68,9 @@
     <t>音效名称</t>
   </si>
   <si>
-    <t xml:space="preserve">循环播放
-0=不循环
-1=循环</t>
+    <t xml:space="preserve">循环次数
+=0 不限次数
+&gt;0 指定次数</t>
   </si>
   <si>
     <t>音量大小</t>
@@ -718,7 +718,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1343,7 +1343,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -1371,7 +1371,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" ht="71.25">
+    <row r="3" ht="85.5">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">

</xml_diff>